<commit_message>
Initial commit - data matching and fusion
</commit_message>
<xml_diff>
--- a/Scraping/Data Sources - scraped/DirektImportWines.xlsx
+++ b/Scraping/Data Sources - scraped/DirektImportWines.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Data Integration\winerecommender\Scraping\Data Sources - scraped\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A5605E-B92B-48A2-ADF7-F17C740E02F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520503CF-378A-4C03-B730-9FAA776D553E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14775" uniqueCount="2943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15274" uniqueCount="3222">
   <si>
     <t>Name:</t>
   </si>
@@ -8854,6 +8855,843 @@
   </si>
   <si>
     <t xml:space="preserve"> Stephan Reinhardt, wine advocate, Dezember 2015: "Intense ripe fruit aromas on the nose of the 2014 Nieder-Florsheim Frauenberg Riesling trocken GG lead to a full-bodied, rich and juicy, well structured but still somewhat unbalanced palate. Its finish is still closed, and somewhat bitter and drying. However, the salinity and intensity are promising; the wine just needs its time."</t>
+  </si>
+  <si>
+    <t>Jahrgang</t>
+  </si>
+  <si>
+    <t>Rebsorte</t>
+  </si>
+  <si>
+    <t>Weingut</t>
+  </si>
+  <si>
+    <t>Produktbezeichnung</t>
+  </si>
+  <si>
+    <t>Winzer</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Charakteristik</t>
+  </si>
+  <si>
+    <t>2016 Cascina Castlèt Passum Barbera d'Asti D.O.C.G. Superiore 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>Barbera</t>
+  </si>
+  <si>
+    <t>Cascina Castlet</t>
+  </si>
+  <si>
+    <t>Cascina Castlèt Passum Barbera d'Asti D.O.C.G. Superiore</t>
+  </si>
+  <si>
+    <t>Dunkles Fleisch, Wildgeflügel, Hartkäse, Risotto, Trüffel, Vorspeise</t>
+  </si>
+  <si>
+    <t>Italien</t>
+  </si>
+  <si>
+    <t>Maria &amp; Ada Borio</t>
+  </si>
+  <si>
+    <t>Piemont</t>
+  </si>
+  <si>
+    <t>Rotwein</t>
+  </si>
+  <si>
+    <t>trocken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dieser Barbera steht in einer Reihe mit Barolo und Barbaresco. Ein Triumph der traditionellen roten Rebe Piemonts!  Ein Symbol, vielleicht ein "Mandala", vielleicht ein antikes "P", vielleicht eine Sonne, direkt im Siebdruckverfahren auf das Glas gebrannt, unvergänglich, wie die Erinnerung an diesen Wein selbst. Ein Zeichen, ein Symbol zeitloser Überlieferung und zugleich grafischer Aktualität. Der Name ruft einige berühmte Weine aus der Antike ins Gedächtnis, die aus überreifen oder leicht angetrockneten ("passito") Trauben hergestellt wurden. Die Tradition des aus angetrockneten Trauben hergestellten Barbera ist im Astigiano alt. Es wurden stets nur die allerbesten Trauben dafür verwendet. Der Passum ist heute das Flaggschiff von Cascina Castlèt, da er einerseits ausschliesslich aus der wichtigsten Rebsorte der Gegend hergestellt wird, andererseits eine sehr moderne Interpretation des Althergebrachten darstellt und damit zeigt, dass es auch in an sich armer bäuerlicher Tradition immer ein Eliteprodukt gab. Der Wein ist von intensiv granatroter Farbe. Ein reiches, elegantes und langanhaltendes Bouquet ruft Pflaumen- und Johannesbeer-Konfitüre in den Sinn. Herb, nobel, warm, samtig im Geschmack, womit Wucht und Konzentration des Weines hervorgehoben werden. Ausgeglichenheit und große Harmonie werden einerseits durch milde Tannine unterstrichen, die zur Süsse neigen und andererseits durch einen unaufdringlichen Säuregehalt. Das Anhalten des Aromas ist lang und intensiv, ein besonderes Merkmal für große Weine, die sich zur langen Lagerung eignen. Herkunftsland: Italien. Enthält Sulfite. Alkoholgehalt: 14,5%Vol. Verantwortlicher Lebensmittelunternehmer: Cascina Castlèt | Strada Castelletto 6 | I-14055 Costigliole d'Asti (AT) </t>
+  </si>
+  <si>
+    <t>2017 Cascina Castlèt Litina Barbera d'Asti D.O.C.G. Superiore 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>2011 Cascina Castlèt Barbera d'Asti Superiore</t>
+  </si>
+  <si>
+    <t>Dunkles Fleisch, Wildgeflügel, Risotto, Trüffel, Vegetarisch, Vorspeise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Zeichen der drei "C": Litina, der köstliche Barbera Superiore aus dem Herzen des Piemonts! Der Barbera d'Asti Superiore "Litina" ist der einzige Wein, der auf dem Etikett das Markenzeichen des Hauses trägt: die drei "C", Anfangsbuchstaben von Cascina Castlèt Costigliole d'Asti. Eine bereits verstorbene Großtante, Litina war ihr Name, brachte seinerzeit den Weinberg, der heute ihren Namen trägt, als Mitgift mit - eine weitere Episode in der weiblich geprägten Geschichte des Weingutes, das heute von Ada und Mariuccia Borio geführt wird. Litina ist das Herz des Weingutes, der perfekte Botschafter für das Piemont und darüber hinaus ein großartiger Rotwein. Intensiv rubinrot, nach längerer Lagerung zu granatrot neigend. Reichhaltiges Bouquet von Waldbeeren, dunklen Steinfrüchten und etwas Vanille. Trocken, warm im Geschmack, körperreich und gut strukturiert, hebt er die Typizität der Rebsorte besonders hervor. Großartig vollmundig und ausgewogen, lang und intensiv anhaltend. Sichern Sie sich die Jubiläumsausgabe "50 Anni": vor 50 Jahren hat Mariuccia ihren ersten Wein bereitet - natürlich Barbera Superiore Litina! </t>
+  </si>
+  <si>
+    <t>2017 Cascina Castlèt Passum Barbera d'Asti D.O.C.G. Superiore</t>
+  </si>
+  <si>
+    <t>2017 Cascina Castlèt Litina Barbera d'Asti D.O.C.G. Superiore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Zeichen der drei "C": Litina, der köstliche Barbera Superiore aus dem Herzen des Piemonts! Der Barbera d'Asti Superiore "Litina" ist der einzige Wein, der auf dem Etikett das Markenzeichen des Hauses trägt: die drei "C", Anfangsbuchstaben von Cascina Castlèt Costigliole d'Asti. Eine bereits verstorbene Großtante, Litina war ihr Name, brachte seinerzeit den Weinberg, der heute ihren Namen trägt, als Mitgift mit - eine weitere Episode in der weiblich geprägten Geschichte des Weingutes, das heute von Ada und Mariuccia Borio geführt wird. Litina ist das Herz des Weingutes, der perfekte Botschafter für das Piemont und darüber hinaus ein großartiger Rotwein. Intensiv rubinrot, nach längerer Lagerung zu granatrot neigend. Reichhaltiges Bouquet von Waldbeeren, dunklen Steinfrüchten und etwas Vanille. Trocken, warm im Geschmack, körperreich und gut strukturiert, hebt er die Typizität der Rebsorte besonders hervor. Großartig vollmundig und ausgewogen, lang und intensiv anhaltend. Sichern Sie sich die Jubiläumsausgabe "50 Anni": vor 50 Jahren hat Mariuccia ihren ersten Wein bereitet - natürlich Barbera Superiore Litina! Herkunftsland: Italien. Enthält Sulfite. Alkoholgehalt: 14,5%Vol. Verantwortlicher Lebensmittelunternehmer: Cascina Castlèt | Strada Castelletto 6 | I-14055 Costigliole d'Asti (AT) </t>
+  </si>
+  <si>
+    <t>2020 Nicolas Duffour Le Galopin de Gascogne Rouge I.G.P.</t>
+  </si>
+  <si>
+    <t>Cabernet Sauvignon, Merlot, Tannat</t>
+  </si>
+  <si>
+    <t>Frankreich</t>
+  </si>
+  <si>
+    <t>Gascogne</t>
+  </si>
+  <si>
+    <t>Roséwein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Neu bei divino: Die drei Schlingel aus der Gascogne "Le Galopin", zu Deutsch "Der Schlingel": Das ist der Name der drei neuen divino Weine in weiß, rosé und rot von Nicolas Duffour aus dem Gers in der Gascogne. Die Landschaft befindet sich am nördlchen Pyrenäenrand und bietet ein einmaliges Terroir, liegt sie doch nicht nur im Klimakorridor zwischen Atlantik und Mittelmeer, sondern stellt für den Weinbau auch verschiedene Lehm- und Kalkböden in mehreren Höhenstufen zur Verfügung. Der Galopin Rouge übersetzt die Tugenden der beiden Brüder ins Rote: Ein frischer, junger Rotwein, der gern gekühlt getrunken werden darf. Die Assemblage ist 25% Merlot, 25% Cabernet Sauvignon und 50% Tannat, eine alte, tanninreiche und himbeerfruchtige Rebsorte aus den Pyrenäen, die dem Wein seinen unverwechsaelbaren Charakter verleiht. Wein aus Frankreich. Enthält Sulfite. Alkoholgehalt: 13,5%Vol. Verantwortlicher Lebensmittelunternehmer: Nicolas Duffour | Domaine Saint-Lannes | F-32330 Lagraulet-du-Gers   </t>
+  </si>
+  <si>
+    <t>2016 Château Godard Bellevue Francs Côtes de Bordeaux A.C. Rouge</t>
+  </si>
+  <si>
+    <t>Cabernet Franc, Cabernet Sauvignon, Merlot</t>
+  </si>
+  <si>
+    <t>Bordeaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neu bei divino: Château Godard Bellevue - ein feiner, Merlot-dominierter Bordeaux aus Francs! Francs ist eine kleinere Bordeaux-Apellationen östlich von Libourne. Traditionell wird hier im Merlot-dominierten Stil, ähnlich wie in den benachbarten Pomerol, Sain-Émilion und Montagne, gearbeitet. Bernadette und Joseph Arbo, die Eltern von Dorian Arbo, keltern auf ihren beiden Liegenschaften (die Châteaux Puyanché und Godard Bellevue), fünf verschiedene Rotweine, dazu einen Weißwein und einen Rosé. Der 2016er Château Godard Bellevue ist ein von 35 bis 45 Jahre alten Rebstöcken gelesener Bordeaux aus 65% Merlot, 20% Cabernet Franc und 15% Cabernet Sauvignon. Der Ausbau erfolgt über 12 Monate in Barriques, davon 30% neu. Die feine Nase zeigt dunkle, reife Würze mit Anklängen von Wacholder, Piment und Zeder, dazu Wildkirsche und Cassis. Am Gaumen mittelschwer mit schöner Mundfülle und nicht überreifer Frucht, wirkt der Wein trotz der griffigen Tannine saftig und elegant, wozu der warme, anhaltende Abgang beiträgt. Ein typischer Merlot-Bordeaux, an dem Sie noch viele Jahre Freude haben werden! </t>
+  </si>
+  <si>
+    <t>2019 Château Arbo Bordeaux A.O.C. Montagne-Saint-Émilion</t>
+  </si>
+  <si>
+    <t>Cabernet Franc, Merlot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exklusiv für Deutschland: Ein umwerfender Spitzen-Bordeaux aus Montagne-Saint-Émilion! Astrid Jordana und Dorian Arbo, beide Winzerfamilien entsprossen, konnten sich mit der Restaurierung und Reaktivierung dieses Mini-Weingutes (nur 8.000 Flaschen in 2018!) in den Hügeln über Saint-Émilion einen Traum erfüllen. Mit viel Respekt vor der Natur entsteht auf dem wunderschönen Anwesen seit 2015 ein hochklassiger, individueller Rotwein. Der 2019er ist ein spät gelesener, kraftvoller Bordeaux aus 88% Merlot und 12% Cabernet Franc, der aufgrund seiner Intensität einen 14-monatigem Ausbau je zur Hälfte in neuen und bereits verwendeten Barriques ermöglichte. Die intensive, komplexe Nase zeigt sofort die typischen Aromen des Merlots: Minze, viel reife rote Beeren, Pflaume, im Hintergrund Andeutungen von Tabak, Kaffee, Schokolade. Am Gaumen entfaltet sich eine reichaltige, elegante Mundfülle, die trotz der Extraktreichheit durchaus opulent, jedoch niemals marmeladig oder zu üppig wirkt.  Trotz seiner Jugend ist der Château Arbo, aufgrund der gut gelungenen Einbindung der kräftigen Tannine, bereits jetzt mit Genuss trinkbar und verspricht für die nächsten zehn bis fünfzehn Jahre eine wundervolle Reifung zu einem glorreichen Vin de Garde. Durch persönliche Vermittlung bin ich an eine Probeflasche dieses besonderen Rotweines gekommen und war sofort überzeugt, wieder einmal eine Perle für das divino-Sortiment aufgetan zu haben. Profitieren Sie jetzt von dem äußerst günstigen Einführungspreis dieses außergewöhnlichen Weines! Herkunftsland: Frankreich. Enthält Sulfite. Alkoholgehalt: 15,0%Vol. Verantwortlicher Lebensmittelunternehmer: Château Arbo | EARL Jorda | Route des Faucheries 13 | F-33570 Montagne Château Arbo </t>
+  </si>
+  <si>
+    <t>2020 Cantina Trerè Cà More Ravenna Rosso I.G.T.</t>
+  </si>
+  <si>
+    <t>Emilia-Romagna</t>
+  </si>
+  <si>
+    <t>Weißwein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">divino goes Romagna: Trerè - die heiligen drei (Wein-) Könige aus dem ravennatischen Apennin! Die Familie Trerè besitzt 35 Hektar Weinberge in den Hügeln westlich von Faenza. Neben der Weinerzeugung wird noch ein kleiner Agriturismo betrieben. L'Arte del Vino - das ist der Claim von Morena und ihrem Sohn Massimo. Dementsprechend wurden auch die Flaschenetiketten von der Künstlerin Jona Sbarzaglia gestaltet. Das lebendige, vielversprechende Rubinrot dieses ungewöhnlichen Tropfens weckt sofort Assoziationen mit toskanischen Rotweinen - nicht von ungefähr, denn schließlich wird der Cà More aus je 50% Sangiovese und Syrah bereitet. Der Sangiovese verleiht der Cuvée die reifen, delikaten und eleganten Beerennoten, allen voran Kirsche, der Syrah die feine, kühle Würze und Vollmundigkeit. Das Ergebins ist ein reichhaltiger, einladender Rotwein voller wohlmeinender Gefälligkeit - im besten Sinne. Gönnt Euch das! Tipp: wer den Cà More mindestens zwei Stunden vor dem Genuss öffnet, wird mit einem besonders feinen, nuancenreichen Bukett und milder, weiniger Mundfülle belohnt. </t>
+  </si>
+  <si>
+    <t>2019 Hermanos del Villar Gaudeamus Roble D.O. Ribera del Duero</t>
+  </si>
+  <si>
+    <t>Tempranillo</t>
+  </si>
+  <si>
+    <t>Spanien</t>
+  </si>
+  <si>
+    <t>Ribera del Duero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Von Rueda ins Duero-Tal: der Ausflug hat sich gelohnt! Tatsächlich: Originär stammt Hermanos del Villar aus Rueda, wo allerdings ausschließlich hervorragende Weißweine aus Verdejo und Sauvignon Blanc bereitet werden. Nun wollte Pablo del Villar sein Portfolio jedoch um einen schönen Rotwein erweitern. Was liegt da näher, als das benachbarte Tempranillo-Paradies Ribera del Duero? Hier ist er also, Gaudeamus, der erste Rotwein des Hauses: Ein Tinto Roble aus 100% Tempranillo, wegen der nur fünfmonatigen Barriquelagerung (je 1/3 der Marge in neuen, ein- bzw. zweijährigen Fässern) auch Semicrianza genannt. Das Ergebnis überzeugt sofort: voluminös, aber nicht fettig, in der Nase intensive Aromen nach dunklen, reifen Beeren, gepaart mit ganz milden Barriquetönen, am Gaumen vollmundig, fruchtig, mit sanften, gut eingebundenen Tanninen und leichter Mineralität. Das leckere Tröpfchen ist bereits erstaunlich reif und wird sich bestimmt noch weitere drei Jahre halten. Ich freue mich, Ihnen diesen wundervollen Rotwein zu einem besonders interessanten Preis anbieten zu können. Oder, wie der Lateiner sagt: Gaudeamus! Herkunftsland: Spanien. Enthält Sulfite. Alkoholgehalt: 13,5%Vol. Verantwortlicher Lebensmittelunternehmer: Hnos. del Villar | Calle Zarzillo | E-47490 Rueda </t>
+  </si>
+  <si>
+    <t>2018 Teanum ÒTRE Negroamaro "Fish"</t>
+  </si>
+  <si>
+    <t>Negroamaro</t>
+  </si>
+  <si>
+    <t>Cantina Teanum</t>
+  </si>
+  <si>
+    <t>2013 Teanum ÒTRE Negroamaro</t>
+  </si>
+  <si>
+    <t>Fisch, Meeresfrüchte, Weichkäse</t>
+  </si>
+  <si>
+    <t>Teanum</t>
+  </si>
+  <si>
+    <t>Apulien</t>
+  </si>
+  <si>
+    <t>leichter Wein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teanum reaktiviert eine alte Tradition - leichter Rotwein statt Weißwein! Die Cantina Teanum ist eine ehemalige Winzervereinigung unter neuer Leitung - das junge Önologenteam bringt frischen Wind in die mittlerweile doch recht angestaubte Weinlandschaft Apuliens! Der Negroamaro wird nur sieben Tage auf der Maische belassen, dadurch ist er praktisch tanninfrei. Danach wird er im Grunde wie ein Weißwein behandelt. Das Ergebnis ist ein durchaus kühl zu trinkender, frisch-saftiger Rotwein, der sich beispielsweise gut zum Grillabend, zu kräftigem Fisch mit Kräutern oder zu Tapas eignet. Im Gegensatz zu leichten roten Norditalieneren fehlen ihm glücklicherweise komplett die Bittertöne von Bardolino, Valpolicella und Co; der Negroamaro ist darüber hinaus deutlich vollmundiger. </t>
+  </si>
+  <si>
+    <t>2018 Teanum ÒTRE Nero di Troia</t>
+  </si>
+  <si>
+    <t>Nero di Troia</t>
+  </si>
+  <si>
+    <t>Teanum ÒTRE Nero di Troia</t>
+  </si>
+  <si>
+    <t>Dunkles Fleisch, Wildgeflügel, Hartkäse, Steak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der nächste Streich von Teanum: Nero di Troia in der ÒTRE-Variante!  Angeblich soll diese rotschalige Rebsorte aus dem antiken hellenischen Troja stammen, aber gewiss ist hier die nahe Foggia liegende Stadt Troia Namensgeber gewesen. Rubinrot und nach reifen roten Früchten duftend kommt der Nero di Troia ins Glas. Reichhaltig und vollmundig am Gaumen, mit Aromen nach Karamell, Vanille und Pflaume, gefällt der Wein besonders durch die gut eingebundenen, milden Tannine und die feinen Reifetöne. Gewiss der klassischste Rotwein aus dem Hause Teanum und damit ie passende Alternative zum berühmten Primitivo! </t>
+  </si>
+  <si>
+    <t>2018 Teanum VENTO Rosso Nero di Troia &amp; Primitivo</t>
+  </si>
+  <si>
+    <t>Primitivo</t>
+  </si>
+  <si>
+    <t>2013 Teanum VENTO Rosso Nero di Troia &amp; Primitivo</t>
+  </si>
+  <si>
+    <t>Pasta, Vegetarisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aller guten Dinge sind drei: Als Weiß, - Rosé oder Rotwein bringt VENTO frischen Wind in die verstaubte Weinlandschaft Apuliens! VENTO, das junge Projekt des Önologen-Teams von Teanum, sind Weine aus autochthonen Rebsorten Apuliens. Der Rotwein wird aus Nero di Troia und Primitivo bereitet. Trotz aller Dichte und Konzentration der reifen Frucht- und Marmeladearomen erscheint der Wein überraschend leichtfüßig am Gaumen. In Verbindung mit den weichen und eleganten Tanninen entsteht so ein niemals schwerer Wein, der durchaus auch angekühlt genossen werden kann. Wir freuen uns, Ihnen den VENTO von Teanum zu einem ganz besonders interessanten Preis anbieten zu können! </t>
+  </si>
+  <si>
+    <t>2019 Domaine Grand Veneur Côtes du Rhône A.C. Les Champauvins</t>
+  </si>
+  <si>
+    <t>Grenache, Mouvèdre</t>
+  </si>
+  <si>
+    <t>Domaine Grand Veneur</t>
+  </si>
+  <si>
+    <t>2012 Domaine Grand Veneur Côtes du Rhône A.C. Les Champauvins</t>
+  </si>
+  <si>
+    <t>Christophe &amp; Sebastien Jaume</t>
+  </si>
+  <si>
+    <t>Côtes du Rhône</t>
+  </si>
+  <si>
+    <t>intensiver, nicht schwerer Wein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quasi ein kleiner Châteauneuf-du-Pape mit allen Genen des großen Bruders Aus 70% Grenache, 20% Syrah und 10% Mouvèdre wird dieser Côtes du Rhône aus Orange gekeltert, gelesen von im Schnitt 60 Jahre alten Rebstöcken, angebaut auf einer direkt an die Châteauneuf-du-Pape-Zone angrenzenden Parzelle. Der Ertrag ist auf lediglch 34hl/ha beschränkt. Demensprechend kräftig, elegant, beerenfruchtig, voluminös und würzig kommt der Wein ins Glas. Da der "Les Champauvins" etwas früher als die berühmten Verwandten ausreift, ist er bereits drei bis vier Jahre nach der Lese mit Genuss zu trinken und hat noch weitere drei bis vier Jahre Entwicklungspotenzial. Damit passt dieser großartige Wein perfekt zur Understatement-Philosophie des Hauses Jaume! Herkunftsland: Frankreich. Enthält Sulfite. Alkoholgehalt: 14,5%Vol. Verantwortlicher Lebensmittelunternehmer: Vignobles Alain Jaume | Domaine Grand Veneur | Route de Châteauneuf-du-Pape 1358 | F-84100 Orange </t>
+  </si>
+  <si>
+    <t>2017 Domaine Grand Veneur "Le Miocène" Châteauneuf-du-Pape A.C. 0,375l</t>
+  </si>
+  <si>
+    <t>Grenache, Mouvèdre, Shiraz / Syrah</t>
+  </si>
+  <si>
+    <t>Domaine Grand Veneur Blanc de Viognier A.C.amd Veneur "Le Miocène" Châteauneuf-du-Pape 0,375l</t>
+  </si>
+  <si>
+    <t>Dunkles Fleisch, Wildgeflügel</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape</t>
+  </si>
+  <si>
+    <t>extraktreicher, schwerer Wein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neben Gigondas und Vacqueyras einer der drei großen Südfranzosen und gleichzeitig eine gute Investition in die Zukunft! Nach einigen umstrittenen Jahren, in denen sich die Jaumes, vor allem beim 2002, dennoch wacker geschlagen haben, ist seit 2005 wieder ein guter Jahrgang nach dem anderen zu verzeichnen. Der Châteauneuf-du-Pape von Jaume aus 50% Grenache, 30% Syrah und 20% Mouvèdre ist jedenfalls so wuchtig, konzentriert, tief dunkelbeerenfruchtig, leicht würzig und lang im Abgang, wie er sein soll. Für den perfekten Genuss benötigt dieser Wein leider noch mindestens zwei Jahre Flaschenreife. Die Wartezeit versüßen Sie sich am besten mit dem Côtes du Rhône Villages Les Champauvins aus gleichem Hause... Herkunftsland: Frankreich. Enthält Sulfite. Alkoholgehalt: 14,0%Vol. Verantwortlicher Lebensmittelunternehmer: Vignobles Alain Jaume | Domaine Grand Veneur | Route de Châteauneuf-du-Pape 1358 | F-84100 Orange </t>
+  </si>
+  <si>
+    <t>2019 Domaine Girard Tradition Rouge A.O.P. Malepère</t>
+  </si>
+  <si>
+    <t>Pinot Noir / Spätburgunder</t>
+  </si>
+  <si>
+    <t>Domaine Girard</t>
+  </si>
+  <si>
+    <t>Domaine Girard Pinot Noir</t>
+  </si>
+  <si>
+    <t>Dunkles Fleisch, Wildgeflügel, Helles Fleisch, Geflügel, Weichkäse</t>
+  </si>
+  <si>
+    <t>Philippe Girard</t>
+  </si>
+  <si>
+    <t>Languedoc-Roussillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malepère Tradition oder ein milder Bordeaux Style Blend? Alles eine Frage der Perspektive! Die Domaine Girard liegt südwestlich von Carcassonne und westlich von Limoux im Örtchen Alaigne, Gemeinde der winzig kleinen A.O.C. Malepère im Languedoc-Roussillon. Die Besonderheit der Gegend ist das Zusammenspiel dreier klimatischer Einflüsse: vor Ort die kühle Höhenlage, von Westen frisches atlantisches Klima und von Osten warme mediterrane Luft. Philippe Girard, Winzer in fünfter Generation, bereitet seinen Tradition Rouge aus 40% Cabernet Franc und 60% Merlot. Der Wein wird bewusst nur im Stahltank ausgebaut, um die feine Mineralität, die der karge Kalksteinboden dem Wein verleiht, zu bewahren. Diese Besonderheit, gepaart mit den rebsortentypischen Aromen von dunklem Steinobst und roten Beeren, ergibt einen einen eleganten Rotwein für jede Gelegenheit, der jetzt bereits gut trinkbar ist, aber auch noch ein paar Jahre aquf der Flasche haben darf. </t>
+  </si>
+  <si>
+    <t>2019 Rejadorada Tinto Roble D.O. Toro 0,375l</t>
+  </si>
+  <si>
+    <t>Tinto del Toro</t>
+  </si>
+  <si>
+    <t>Toro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die rassige Semicrianza aus der aufstrebenden Mini-D.O. Toro Die kleine Bodega Rejadoara ("Goldenes Gitter") liegt in der hierzulande relativ unbekannten D.O. Toro in der nordwestspanischen Region Kastilien &amp; Léon. Benavente, Rueda und Ribera del Duero sind hier nicht nur geographisch, sondern auch kulturell näher als Navarra und Rioja. Seit 2015 gehören die Weine von Mario Remesal zum Portfolio von divino Weinhandel.  Marios Tinto Roble bekommt sechs Monate Barriquereife, also einen Monat mehr, als gesetzlich vorgeschrieben, spendiert. Damit ist er eigentlich bereits eine Semicrianza. In die ausschließlich neuen Barrique-Fässer kommt zu 100% Tempranillo, hier als lokale Spielart „Tinta de Toro“. Das Ergebnis kann sich sehen lassen: da kommt ein dunkelroter, extraktreicher Wein mit rebsortentypisch purpurfarbenen Reflexen ins Glas. In der Nase reichhaltige, reife Aromen nach Maulbeere und Brombeere. Am Gaumen intensiv fruchtig, mit kraftvollen, aber gut eingebundenen Tanninen und Barriquetönen. Lang anhaltender Abgang. Insgesamt ein charakterstarker „Vin de Garde“ zu einem auffallend maßvollen Preis. Der Rejadorada Tinto Roble D.O. Toro hat mindestens noch fünf bis sechs Jahre Reifepotenzial. Zur Einlagerung empfehle ich die ebenfalls erhältliche Magnum-Variante. </t>
+  </si>
+  <si>
+    <t>2016 Rejadorada Novellum Crianza D.O. Toro Magnum (1,5l)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spitzen-Crianza aus der aufstrebenden D.O. Toro Die kleine Bodega Rejadoara ("Goldenes Gitter") liegt in der hierzulande relativ unbekannten D.O. Toro in der nordwestspanischen Region Kastilien &amp; Léon. Benavente, Rueda und Ribera del Duero sind hier nicht nur geographisch, sondern auch kulturell näher als Navarra und Rioja. Seit 2015 gehören die Weine von Mario Remesal zum Portfolio von divino Weinhandel.  Das kleine, qualitätsversessene Weingut bietet in jeder der spanischen Prädikatsklassen außergewöhnlich gut gelungene Rotweine. Nach Reja Joven und Rejadorada Roble folgt nun die edle Crianza namens Novellum. Die Trauben werden von Hand gelesen. Das Alter der Rebstöcke beträgt zwischen 25 und 50 Jahre. Nach langsamer, bei moderaten 23°C durchgeführter Maischegärung erfolgt der mindestens 12-monatige Ausbau in Barriques aus französischer und amerikanischer Eiche. Danach gönnt Mario seiner Bilderbuch-Crianza noch mindestens zwei weitere Jahre Ruhe auf der Flasche.  Der Wein kommt kirschrot mit rubinroten Reflexen ins Glas. Die komplexe Nase kombiniert reife Aromen von dunklen Beeren mit feinen Anklängen an getoastetes Holz und Lorbeer. Am Gaumen zeigt sich die Novellum Crianza gut ausbalanciert: elegant, samtig und körperreich mit milder Säure sowie gut eingebundenen Tanninen, gefolgt von einem anhaltenden, seidigen Nachklang. Bereits jetzt mit Genuss trinkbar, lohnt sich die weitere Verfeinerung auf der Flasche noch für mindestens sechs weitere Jahre. </t>
+  </si>
+  <si>
+    <t>2016 Rejadorada Novellum Crianza D.O. Toro</t>
+  </si>
+  <si>
+    <t>2020 Rejadorada Reja Joven D.O. Toro</t>
+  </si>
+  <si>
+    <t>Grenache, Tinto del Toro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der kleine Bruder (oder die kleine Schwester?) von Rejadorada Roble &amp; Novellum Crianza: Ein Rotwein für die milden Tage im Jahr! Die kleine Bodega Rejadoara ("Goldenes Gitter") liegt in der hierzulande relativ unbekannten D.O. Toro in der nordwestspanischen Region Kastilien &amp; Léon. Benavente, Rueda und Ribera del Duero sind hier nicht nur geographisch, sondern auch kulturell näher als Navarra und Rioja. Seit 2015 gehören die Weine von Mario Remesal zum Portfolio von divino Weinhandel.  Dem Stil des Hauses folgend wird der Reja zu 85% aus der Tinta de Toro, einer lokalen Spielart der Tempranillo-Rebe, und 15% Garnacha gekeltert. Als Joven reift der Wein ausschließlich im Stahltank und auf der Flasche. Das Ergebnis ist ein herrlich milder, beeriger Rotwein, nicht zu komplex oder zu konzentriert. Die Betonung auf der Frucht und die weichen Tannine bewahren dem Reja, der im Sommer gern kellerkalt genossen werden darf, seine Leichtigkeit und Eleganz. Ein idealer Tapas- und Terrassenwein, der das ganze Jahr über schmeckt. </t>
+  </si>
+  <si>
+    <t>2019 Rejadorada Tinto Roble D.O. Toro</t>
+  </si>
+  <si>
+    <t>2017 Domaine Grand Veneur Châteauneuf-du-Pape A.C. "Les Origines" 1,5l Magnum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Flagschiff aus dem Hause Jaume Dieser Wein setzt Maßstäbe!  Aus 50% Grenache, 20% Syrah und 30% Mourvèdre keltern Christophe und Sébastien Jaume "ihren" Wein - und gewiss hat Vater Alain auch noch die Finger im Spiel. Von den Hängen zwischen Orange und Châteauneuf-du-Pape stammen die Beeren. Der Boden ist hier rötlich, karg und mit viel Geröll durchsetzt - perfekt für tief wurzelnde Reben, die viel Terroir in den Wein bringen. Les Origines ist konzentriert, dunkel, wuchtig und extrem aromatisch. Christophe empfiehlt, den Wein auch in jungen Jahren zu probieren, um ihn in all seinen Entwicklungsstadien zu erleben. Herkunftsland: Frankreich. Enthält Sulfite. Alkoholgehalt: 15,0%Vol. Verantwortlicher Lebensmittelunternehmer: Vignobles Alain Jaume | DOmaine Grand Veneur | Route de Châteauneuf-du-Pape 1358 | F-84100 Orange </t>
+  </si>
+  <si>
+    <t>2018 Domaine Grand Veneur Côtes du Rhône A.C. Les Champauvins 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>2019 Alain Jaume &amp; Fils (Domaine Grand Veneur) Gigondas A.C. Terrasses de Montmirail</t>
+  </si>
+  <si>
+    <t>Alain Jaume Gigondas A.C. Terrasses de Montmirail</t>
+  </si>
+  <si>
+    <t>2018 Alain Jaume &amp; Fils (Domaine Grand Veneur) Vacqueyras A.C. La Grande Garrigue</t>
+  </si>
+  <si>
+    <t>Alain Jaume Vacqueyras La Grande Garrigue</t>
+  </si>
+  <si>
+    <t>2018 Domaine Grand Veneur Châteauneuf-du-Pape A.C. "Les Origines"</t>
+  </si>
+  <si>
+    <t>2011 Domaine Grand Veneur Châteauneuf-du-Pape "Les Origines"</t>
+  </si>
+  <si>
+    <t>2013 Le Lame Sorripa Chianti Classico D.O.C.G. Gallo Nero Gran Selezione</t>
+  </si>
+  <si>
+    <t>Tenuta Le Lame</t>
+  </si>
+  <si>
+    <t>Le Lame Chianti Classico Gallo Nero Riserva</t>
+  </si>
+  <si>
+    <t>Mario Zanobini</t>
+  </si>
+  <si>
+    <t>2015 Le Lame Chianti Classico D.O.C.G. Gallo Nero Riserva</t>
+  </si>
+  <si>
+    <t>2016 Le Lame Chianti Classico D.O.C.G. Gallo Nero</t>
+  </si>
+  <si>
+    <t>Le Lame Chianti Classico Gallo Nero</t>
+  </si>
+  <si>
+    <t>2019 Cascina Castlèt "Vespa" Barbera d'Asti D.O.C.G.</t>
+  </si>
+  <si>
+    <t>Cascina Castlèt "Vespa" Barbera d'Asti D.O.C.G.</t>
+  </si>
+  <si>
+    <t>2019 Cascina Castlèt "Vespa" Barbera d'Asti D.O.C.G. 0,375l</t>
+  </si>
+  <si>
+    <t>2019 Teanum ÒTRE Primitivo I.G.T. Puglia</t>
+  </si>
+  <si>
+    <t>Teanum Òtre Primitivo</t>
+  </si>
+  <si>
+    <t>2015 Rignana Chianti Classico D.O.C.G. Gallo Nero Gran Selezione</t>
+  </si>
+  <si>
+    <t>Fattoria di Rignana</t>
+  </si>
+  <si>
+    <t>Rignana Chianti Classico Gallo Nero Riserva</t>
+  </si>
+  <si>
+    <t>Cosimo Gericke</t>
+  </si>
+  <si>
+    <t>2018 Rignana Le Villane Rosso Toscano I.G.T.</t>
+  </si>
+  <si>
+    <t>Rignana Chianti Classico Gallo Nero</t>
+  </si>
+  <si>
+    <t>2016 Rignana Chianti Classico D.O.C.G. Gallo Nero Riserva</t>
+  </si>
+  <si>
+    <t>2018 Rignana Chianti Classico D.O.C.G. Gallo Nero</t>
+  </si>
+  <si>
+    <t>2013 Cantina di Venosa Carato Venusio D.O.C.G. Aglianico del Vulture 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>2018 Château Arbo Bordeaux A.O.C. Montagne-Saint-Émilion</t>
+  </si>
+  <si>
+    <t>2018 Château Arbo Bordeaux A.O.C. Montagne-Saint-Émilion 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>2014 Otero Reserva D.O.P. Valles de Benavente</t>
+  </si>
+  <si>
+    <t>2015 Otero Crianza D.O.P. Valles de Benavente</t>
+  </si>
+  <si>
+    <t>2019 Grand Veneur Côtes du Rhône A.C. Rouge</t>
+  </si>
+  <si>
+    <t>Réserve Grand Veneur Côtes du Rhône A.C.</t>
+  </si>
+  <si>
+    <t>2018 Cantina di Venosa Verbo Rosso D.O.P. Aglianico del Vulture</t>
+  </si>
+  <si>
+    <t>2014 Teanum Gran Tiati</t>
+  </si>
+  <si>
+    <t>Teanum Gran Tiati</t>
+  </si>
+  <si>
+    <t>2018 Domaine Girard Cuvée Neri Rouge A.O.P. Malepère Magnum (1,5l)</t>
+  </si>
+  <si>
+    <t>Domaine Girard Cuvée Neri</t>
+  </si>
+  <si>
+    <t>2018 Domaine Girard Cuvée Neri Rouge A.O.P. Malepère</t>
+  </si>
+  <si>
+    <t>2018 Domaine Girard Pinot Noir I.G.P.</t>
+  </si>
+  <si>
+    <t>2019 Alain Jaume &amp; Fils (Domaine Grand Veneur) Ventoux A.C. "Les Gélinottes"</t>
+  </si>
+  <si>
+    <t>Alain Jaumes Ventoux "Les Gélinottes"</t>
+  </si>
+  <si>
+    <t>2019 Grand Veneur Côtes du Rhône A.C. Rouge 0,375l</t>
+  </si>
+  <si>
+    <t>Réserve Grand Veneur Côtes du Rhône Rouge 0,375l</t>
+  </si>
+  <si>
+    <t>2013 Cantina di Venosa Carato Venusio D.O.C.G. Aglianico del Vulture Superiore</t>
+  </si>
+  <si>
+    <t>2018 Cantina di Venosa Terre di Orazio D.O.P. Aglianico del Vulture</t>
+  </si>
+  <si>
+    <t>2019 Cantina di Venosa Matematico Merlot Vino Rosso Vulcanico</t>
+  </si>
+  <si>
+    <t>2016 Château Arbo Bordeaux A.O.C. Montagne-Saint-Émilion 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>2016 Château Arbo Bordeaux A.O.C. Montagne-Saint-Émilion</t>
+  </si>
+  <si>
+    <t>2015 Bagordi Crianza D.O.C. Rioja</t>
+  </si>
+  <si>
+    <t>2017 Bagordi Tinto Cosecha 6 Meses Barrica D.O.C. Rioja</t>
+  </si>
+  <si>
+    <t>2016 Château La Fleur Lauga Bordeaux A.O.C. Saint-Julien Cru Artisan</t>
+  </si>
+  <si>
+    <t>2016 La Petite Fleur de Château La Fleur Lauga Bordeaux A.O.C. Saint-Julien Cru Artisan</t>
+  </si>
+  <si>
+    <t>2015 Château de Lauga Bordeaux A.O.C. Haut-Médoc Cru Artisan Magnumflasche (1,5l)</t>
+  </si>
+  <si>
+    <t>2016 Château de Lauga Bordeaux A.O.C. Haut-Médoc Cru Artisan 0,375l</t>
+  </si>
+  <si>
+    <t>2016 Château de Lauga Bordeaux A.O.C. Haut-Médoc Cru Artisan</t>
+  </si>
+  <si>
+    <t>2015 Château de Lauga Bordeaux A.O.C. Haut-Médoc Cru Artisan</t>
+  </si>
+  <si>
+    <t>2016 Château de Lauga Bordeaux A.O.C. Haut-Médoc Cru Artisan Magnumflasche (1,5l)</t>
+  </si>
+  <si>
+    <t>2017 Cantina di Venosa Terre di Orazio D.O.P. Aglianico del Vulture 0,375l</t>
+  </si>
+  <si>
+    <t>2017 Cantina di Venosa Gesualdo D.O.P. Aglianico del Vulture</t>
+  </si>
+  <si>
+    <t>2018 Otero Finca Valleoscuro Tinto D.O.P. Valles de Benavente</t>
+  </si>
+  <si>
+    <t>2014 Bagordi Garnacha Crianza D.O.C. Rioja</t>
+  </si>
+  <si>
+    <t>2014 Bagordi Graciano Crianza D.O.C. Rioja</t>
+  </si>
+  <si>
+    <t>2014 Ochoa Tempranillo Crianza D.O. Navarra</t>
+  </si>
+  <si>
+    <t>2012 Ochoa Tempranillo Crianza D.O. Navarra 1,5l Magnum</t>
+  </si>
+  <si>
+    <t>2012 Adriana Ochoa 8A Mil Gracias Graciano Crianza D.O. Navarra</t>
+  </si>
+  <si>
+    <t>2013 Rejadorada Tinto Roble D.O. Toro Magnum (1,5l)</t>
+  </si>
+  <si>
+    <t>2021 Cascina Castlèt Moscato d'Asti D.O.C.G.</t>
+  </si>
+  <si>
+    <t>Cascina Castlèt Moscato d'Asti D.O.C.G.</t>
+  </si>
+  <si>
+    <t>Antech Blanquette de Limoux A.C. Doux et fruité Méthode ancestrale</t>
+  </si>
+  <si>
+    <t>Georges &amp; Roger Antech</t>
+  </si>
+  <si>
+    <t>Antech Blanquette de Limoux Doux et fruité Méthode ancestrale</t>
+  </si>
+  <si>
+    <t>Francoise Antech</t>
+  </si>
+  <si>
+    <t>2021 Teanum VENTO Bianco Falanghina &amp; Chardonnay</t>
+  </si>
+  <si>
+    <t>Teanum Vento Bianco Falanghina &amp; Chardonnay</t>
+  </si>
+  <si>
+    <t>2020 Kassner-Simon Weißer Burgunder Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Kassner-Simon Merlot Blanc de Noir Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Kassner-Simon Grauburgunder Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Kassner-Simon Auxerrois Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Kassner-Simon Riesling Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Weingut Hain Piesporter Riesling Q.b.A. feinherb</t>
+  </si>
+  <si>
+    <t>Weingut Hain</t>
+  </si>
+  <si>
+    <t>Weingut Hain Piesporter Riesling feinherb</t>
+  </si>
+  <si>
+    <t>Gernot Hain</t>
+  </si>
+  <si>
+    <t>2020 Weingut Hain Chardonnay Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>Weingut Hain Chardonnay Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Weingut Hain Piesporter Goldtröpfchen Riesling Kabinett trocken</t>
+  </si>
+  <si>
+    <t>Weingut Hain Piesporter Goldtröpfchen Riesling Kabinett trocken</t>
+  </si>
+  <si>
+    <t>2021 Cantina di Venosa Verbo Bianco Malvasia I.G.P. Basilicata</t>
+  </si>
+  <si>
+    <t>2020 Nicolas Duffour Le Galopin de Gascogne Blanc I.G.P.</t>
+  </si>
+  <si>
+    <t>2020 Nicolas Duffour Les Aubas Sauvignon Blanc &amp; Gros-Manseng Medium I.G.P. Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>2020 Nicolas Duffour Les Aubas Gros-Manseng I.G.P. Côtes de Gascogne</t>
+  </si>
+  <si>
+    <t>2020 Château Puyanché Francs Côtes de Bordeaux A.C. Blanc Sec</t>
+  </si>
+  <si>
+    <t>2020 Domaine Grand Veneur Blanc de Viognier Côtes du Rhône A.C.</t>
+  </si>
+  <si>
+    <t>Domaine Grand Veneur Blanc de Viognier A.C.</t>
+  </si>
+  <si>
+    <t>2020 Grand Veneur Côtes du Rhône A.C. Blanc</t>
+  </si>
+  <si>
+    <t>Réserve Grand Veneur Côtes du Rhône A.C. Blanc</t>
+  </si>
+  <si>
+    <t>2020 Cantina Trerè Giòja Romagna Pagadebit Frizzante D.O.C.</t>
+  </si>
+  <si>
+    <t>2020 Cantina Trerè Rè Famoso Bianco I.G.T. Ravenna</t>
+  </si>
+  <si>
+    <t>2020 Gaggioli Bagazzino Bianco Pignoletto D.O.C.</t>
+  </si>
+  <si>
+    <t>2020 Otero Finca Valleoscuro Blanco D.O.P. Valles de Benavente</t>
+  </si>
+  <si>
+    <t>2020 Hermanos del Villar Oro de Castilla Sauvignon Blanc D.O. Rueda</t>
+  </si>
+  <si>
+    <t>2020 Hermanos del Villar Oro de Castilla Verdejo D.O. Rueda</t>
+  </si>
+  <si>
+    <t>2020 Hermanos del Villar Azoe Verdejo D.O. Rueda</t>
+  </si>
+  <si>
+    <t>2020 Teanum ÒTRE Falanghina I.G.T. Puglia</t>
+  </si>
+  <si>
+    <t>2020 Weingut Hain Weißburgunder Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>Weingut Hain Weißburgunder Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2021 Domaine Girard Chardonnay Classique I.G.P.</t>
+  </si>
+  <si>
+    <t>2020 Weingut Hain Piesporter Riesling Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>Hain Piesporter Riesling trocken</t>
+  </si>
+  <si>
+    <t>2019 Weingut Hain Spätburgunder Blanc de Noir Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>Weingut Hain Spätburgunder Blanc de Noir</t>
+  </si>
+  <si>
+    <t>2019 Weingut Hain Piesporter Riesling Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2019 Weingut Hain Piesporter Goldtröpfchen Riesling Kabinett feinherb</t>
+  </si>
+  <si>
+    <t>2014 Weingut Hain Piesporter Goldtröpfchen Riesling Kabinett feinherb</t>
+  </si>
+  <si>
+    <t>2019 Weingut Hain Piesporter Goldtröpfchen Riesling Alte Reben feinherb</t>
+  </si>
+  <si>
+    <t>2011 Hain Piesporter Goldtröpfchen Spätlese feinherb</t>
+  </si>
+  <si>
+    <t>2019 Cascina Castlèt A Taj Piemonte Chardonnay D.O.C.</t>
+  </si>
+  <si>
+    <t>2012 Cascina Castlèt A Taj Piemonte Chardonnay</t>
+  </si>
+  <si>
+    <t>2019 Grand Veneur Côtes du Rhône A.C. Blanc 0,375l</t>
+  </si>
+  <si>
+    <t>2014 Réserve Grand Veneur Côtes du Rhône Blanc 0,375l</t>
+  </si>
+  <si>
+    <t>2018 Bagordi Blanco D.O.C. Rioja</t>
+  </si>
+  <si>
+    <t>2016 Adriana Ochoa 8A Uva Doble Blanco D.O. Navarra</t>
+  </si>
+  <si>
+    <t>2015 Specogna Friulano D.O.C. Colli Orientali del Friuli</t>
+  </si>
+  <si>
+    <t>Leonardo Specogna</t>
+  </si>
+  <si>
+    <t>Specogna Friulano Colli Orientali del Friuli</t>
+  </si>
+  <si>
+    <t>2014 Specogna Chardonnay D.O.C. Colli Orientali del Friuli</t>
+  </si>
+  <si>
+    <t>Specogna Chardonnay Colli Orientali del Friuli</t>
+  </si>
+  <si>
+    <t>2015 Specogna Pinot Grigio Venezia Giulia</t>
+  </si>
+  <si>
+    <t>Specogna Pinot Grigio Venezia Giulia</t>
+  </si>
+  <si>
+    <t>2015 Specogna Sauvignon D.O.C. Colli Orientali del Friuli</t>
+  </si>
+  <si>
+    <t>Specogna Sauvignon Colli Orientali del Friuli</t>
+  </si>
+  <si>
+    <t>2013 Jean-Pierre Michel Macon Villages A.C. Terroir de Quintaine</t>
+  </si>
+  <si>
+    <t>Jean-Pierre Michel</t>
+  </si>
+  <si>
+    <t>2013 Jean-Pierre Michel Macon Villages Terroir de Quintaine</t>
+  </si>
+  <si>
+    <t>2010 Jean-Pierre Michel Viré-Clessé A.C. Terroirs de Quintaine</t>
+  </si>
+  <si>
+    <t>2010 Jean-Pierre Michel Viré-Clessé Terroirs de Quintaine</t>
+  </si>
+  <si>
+    <t>2014 Antech Crémant de Limoux A.C. Brut Cuvée Elixir</t>
+  </si>
+  <si>
+    <t>Antech Crémanrt de Limoux A.C. Brut Cuvée Elixir</t>
+  </si>
+  <si>
+    <t>2019 Antech Crémant de Limoux Brut Rosé Cuvée Émotion</t>
+  </si>
+  <si>
+    <t>Antech Crémant de Limoux A.C. Brut Rosé Cuvée Émotion</t>
+  </si>
+  <si>
+    <t>2018 Antech Crémant de Limoux Brut A.C. Cuvée Eugenie</t>
+  </si>
+  <si>
+    <t>Antech Crémant de Limoux Brut Cuvée Eugenie</t>
+  </si>
+  <si>
+    <t>2017 Antech Crémant de Limoux A.C. Brut Cuvée Héritage</t>
+  </si>
+  <si>
+    <t>Antech Crémant de Limoux A.C. Brut Cuvée Héritage</t>
+  </si>
+  <si>
+    <t>Casalini "Rovede" Prosecco di Valdobbiadene Spumante D.O.C.G. Superiore Brut</t>
+  </si>
+  <si>
+    <t>Spumanti Casalini</t>
+  </si>
+  <si>
+    <t>Casalini Prosecco di Valdobbiadene Superiore Extra Dry</t>
+  </si>
+  <si>
+    <t>Andrea Casalini</t>
+  </si>
+  <si>
+    <t>Antech Crémant de Limoux Brut A.C. Cuvée Eugenie Magnum (1,5l)</t>
+  </si>
+  <si>
+    <t>Antech Blanquette de Limoux Brut A.C. Cuvée Tradition</t>
+  </si>
+  <si>
+    <t>Antech Blanquette de Limoux Brut Cuvée Tradition</t>
+  </si>
+  <si>
+    <t>Weingut Hain Riesling Sekt Brut</t>
+  </si>
+  <si>
+    <t>Casalini "Cal Busa" Prosecco di Valdobbiadene Spumante D.O.C.G. Superiore Extra Dry Magnum</t>
+  </si>
+  <si>
+    <t>Casalini Prosecco di Valdobbiadene Superiore Extra Dry Magnum</t>
+  </si>
+  <si>
+    <t>Casalini "Cal Busa" Prosecco di Valdobbiadene Spumante D.O.C.G. Superiore Extra Dry</t>
+  </si>
+  <si>
+    <t>divino.de Prosecco D.O.C. Spumante Extra Dry</t>
+  </si>
+  <si>
+    <t>divino.de Prosecco Spumante Extra Dry</t>
+  </si>
+  <si>
+    <t>divino.de Prosecco D.O.C. Frizzante</t>
+  </si>
+  <si>
+    <t>divino.de Prosecco Frizzante</t>
+  </si>
+  <si>
+    <t>2020 Kassner-Simon Euphorie Rosé Q.b.A. trocken</t>
+  </si>
+  <si>
+    <t>2020 Cascina Castlèt Rosè Vino Rosato</t>
+  </si>
+  <si>
+    <t>2020 Nicolas Duffour Le Galopin de Gascogne Rosé I.G.P.</t>
+  </si>
+  <si>
+    <t>2020 Otero Finca Valleoscuro Rosado D.O.P. Valles de Benavente</t>
+  </si>
+  <si>
+    <t>2020 Teanum VENTO Rosato Nero di Troia &amp; Negroamaro</t>
+  </si>
+  <si>
+    <t>Teanum Vento Rosato Nero di Troia &amp; Negroamaro</t>
+  </si>
+  <si>
+    <t>2020 Grand Veneur Côtes du Rhône A.C. Rosé "Bellissimé" 0,375l</t>
+  </si>
+  <si>
+    <t>2014 Réserve Grand Veneur Côtes du Rhône Rosé 0,375l</t>
+  </si>
+  <si>
+    <t>2020 Cantina di Venosa Verbo Rosato I.G.P. Basilicata</t>
+  </si>
+  <si>
+    <t>2020 Weingut Hain Cuvée Rosé Q.b.A.</t>
+  </si>
+  <si>
+    <t>Weingut Hain Cuvée Rosé</t>
+  </si>
+  <si>
+    <t>2021 Domaine Girard Garriguette Rosé I.G.P.</t>
+  </si>
+  <si>
+    <t>2020 Grand Veneur Côtes du Rhône A.C. Rosé "Bellissime"</t>
+  </si>
+  <si>
+    <t>Réserve Grand Veneur Côtes du Rhône Rosé</t>
+  </si>
+  <si>
+    <t>2018 Bagordi Rosado D.O.C. Rioja</t>
   </si>
 </sst>
 </file>
@@ -9197,13 +10035,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD815"/>
+  <dimension ref="A1:AD958"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C799" workbookViewId="0">
+      <selection activeCell="M833" sqref="M833"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="105.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -55160,6 +56003,2004 @@
         <v>2942</v>
       </c>
     </row>
+    <row r="816" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>2951</v>
+      </c>
+      <c r="B816" t="s">
+        <v>2953</v>
+      </c>
+      <c r="C816" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D816" t="s">
+        <v>2958</v>
+      </c>
+      <c r="E816" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F816">
+        <v>2016</v>
+      </c>
+      <c r="G816" t="s">
+        <v>2952</v>
+      </c>
+      <c r="J816" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q816" t="s">
+        <v>2955</v>
+      </c>
+      <c r="AC816" t="s">
+        <v>2961</v>
+      </c>
+    </row>
+    <row r="817" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>2962</v>
+      </c>
+      <c r="B817" t="s">
+        <v>2953</v>
+      </c>
+      <c r="C817" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D817" t="s">
+        <v>2958</v>
+      </c>
+      <c r="E817" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F817">
+        <v>2016</v>
+      </c>
+      <c r="G817" t="s">
+        <v>2952</v>
+      </c>
+      <c r="J817" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q817" t="s">
+        <v>2964</v>
+      </c>
+      <c r="AC817" t="s">
+        <v>2965</v>
+      </c>
+    </row>
+    <row r="818" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B818" t="s">
+        <v>2953</v>
+      </c>
+      <c r="C818" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D818" t="s">
+        <v>2958</v>
+      </c>
+      <c r="E818" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F818">
+        <v>2017</v>
+      </c>
+      <c r="G818" t="s">
+        <v>2952</v>
+      </c>
+      <c r="J818" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q818" t="s">
+        <v>2955</v>
+      </c>
+      <c r="AC818" t="s">
+        <v>2961</v>
+      </c>
+    </row>
+    <row r="819" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>2967</v>
+      </c>
+      <c r="B819" t="s">
+        <v>2953</v>
+      </c>
+      <c r="C819" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D819" t="s">
+        <v>2958</v>
+      </c>
+      <c r="E819" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F819">
+        <v>2017</v>
+      </c>
+      <c r="G819" t="s">
+        <v>2952</v>
+      </c>
+      <c r="J819" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q819" t="s">
+        <v>2964</v>
+      </c>
+      <c r="AC819" t="s">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="820" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>2969</v>
+      </c>
+      <c r="C820" t="s">
+        <v>2971</v>
+      </c>
+      <c r="D820" t="s">
+        <v>2972</v>
+      </c>
+      <c r="E820" t="s">
+        <v>2973</v>
+      </c>
+      <c r="G820" t="s">
+        <v>2970</v>
+      </c>
+      <c r="AC820" t="s">
+        <v>2974</v>
+      </c>
+    </row>
+    <row r="821" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>2975</v>
+      </c>
+      <c r="C821" t="s">
+        <v>2971</v>
+      </c>
+      <c r="D821" t="s">
+        <v>2977</v>
+      </c>
+      <c r="E821" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G821" t="s">
+        <v>2976</v>
+      </c>
+      <c r="AC821" t="s">
+        <v>2978</v>
+      </c>
+    </row>
+    <row r="822" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A822" t="s">
+        <v>2979</v>
+      </c>
+      <c r="C822" t="s">
+        <v>2971</v>
+      </c>
+      <c r="D822" t="s">
+        <v>2977</v>
+      </c>
+      <c r="E822" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G822" t="s">
+        <v>2980</v>
+      </c>
+      <c r="AC822" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="823" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A823" t="s">
+        <v>2982</v>
+      </c>
+      <c r="C823" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D823" t="s">
+        <v>2983</v>
+      </c>
+      <c r="E823" t="s">
+        <v>2984</v>
+      </c>
+      <c r="AC823" t="s">
+        <v>2985</v>
+      </c>
+    </row>
+    <row r="824" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A824" t="s">
+        <v>2986</v>
+      </c>
+      <c r="C824" t="s">
+        <v>2988</v>
+      </c>
+      <c r="D824" t="s">
+        <v>2989</v>
+      </c>
+      <c r="E824" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G824" t="s">
+        <v>2987</v>
+      </c>
+      <c r="AC824" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="825" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A825" t="s">
+        <v>2991</v>
+      </c>
+      <c r="B825" t="s">
+        <v>2993</v>
+      </c>
+      <c r="C825" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D825" t="s">
+        <v>2997</v>
+      </c>
+      <c r="E825" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F825">
+        <v>2018</v>
+      </c>
+      <c r="G825" t="s">
+        <v>2992</v>
+      </c>
+      <c r="J825" t="s">
+        <v>2998</v>
+      </c>
+      <c r="Q825" t="s">
+        <v>2995</v>
+      </c>
+      <c r="AC825" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="826" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A826" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B826" t="s">
+        <v>2993</v>
+      </c>
+      <c r="C826" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D826" t="s">
+        <v>2997</v>
+      </c>
+      <c r="E826" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F826">
+        <v>2018</v>
+      </c>
+      <c r="G826" t="s">
+        <v>3001</v>
+      </c>
+      <c r="J826" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q826" t="s">
+        <v>3003</v>
+      </c>
+      <c r="AC826" t="s">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="827" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A827" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B827" t="s">
+        <v>2993</v>
+      </c>
+      <c r="C827" t="s">
+        <v>2956</v>
+      </c>
+      <c r="D827" t="s">
+        <v>2997</v>
+      </c>
+      <c r="E827" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F827">
+        <v>2018</v>
+      </c>
+      <c r="G827" t="s">
+        <v>3006</v>
+      </c>
+      <c r="J827" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q827" t="s">
+        <v>3008</v>
+      </c>
+      <c r="AC827" t="s">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="828" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A828" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B828" t="s">
+        <v>3012</v>
+      </c>
+      <c r="C828" t="s">
+        <v>2971</v>
+      </c>
+      <c r="D828" t="s">
+        <v>3015</v>
+      </c>
+      <c r="E828" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F828">
+        <v>2017</v>
+      </c>
+      <c r="G828" t="s">
+        <v>3011</v>
+      </c>
+      <c r="J828" t="s">
+        <v>3016</v>
+      </c>
+      <c r="Q828" t="s">
+        <v>3003</v>
+      </c>
+      <c r="AC828" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="829" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A829" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B829" t="s">
+        <v>3012</v>
+      </c>
+      <c r="C829" t="s">
+        <v>2971</v>
+      </c>
+      <c r="D829" t="s">
+        <v>3022</v>
+      </c>
+      <c r="E829" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F829">
+        <v>2017</v>
+      </c>
+      <c r="G829" t="s">
+        <v>3019</v>
+      </c>
+      <c r="J829" t="s">
+        <v>3023</v>
+      </c>
+      <c r="Q829" t="s">
+        <v>3021</v>
+      </c>
+      <c r="AC829" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="830" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A830" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B830" t="s">
+        <v>3027</v>
+      </c>
+      <c r="C830" t="s">
+        <v>2971</v>
+      </c>
+      <c r="D830" t="s">
+        <v>3031</v>
+      </c>
+      <c r="E830" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F830">
+        <v>2018</v>
+      </c>
+      <c r="G830" t="s">
+        <v>3026</v>
+      </c>
+      <c r="J830" t="s">
+        <v>2960</v>
+      </c>
+      <c r="Q830" t="s">
+        <v>3029</v>
+      </c>
+      <c r="AC830" t="s">
+        <v>3032</v>
+      </c>
+    </row>
+    <row r="831" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A831" t="s">
+        <v>3033</v>
+      </c>
+      <c r="C831" t="s">
+        <v>2988</v>
+      </c>
+      <c r="D831" t="s">
+        <v>3035</v>
+      </c>
+      <c r="E831" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G831" t="s">
+        <v>3034</v>
+      </c>
+      <c r="AC831" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="832" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A832" t="s">
+        <v>3037</v>
+      </c>
+      <c r="C832" t="s">
+        <v>2988</v>
+      </c>
+      <c r="D832" t="s">
+        <v>3035</v>
+      </c>
+      <c r="E832" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G832" t="s">
+        <v>3034</v>
+      </c>
+      <c r="AC832" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="833" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A833" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C833" t="s">
+        <v>2988</v>
+      </c>
+      <c r="D833" t="s">
+        <v>3035</v>
+      </c>
+      <c r="E833" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G833" t="s">
+        <v>3034</v>
+      </c>
+      <c r="AC833" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="834" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A834" t="s">
+        <v>3040</v>
+      </c>
+      <c r="C834" t="s">
+        <v>2988</v>
+      </c>
+      <c r="D834" t="s">
+        <v>3035</v>
+      </c>
+      <c r="E834" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G834" t="s">
+        <v>3041</v>
+      </c>
+      <c r="AC834" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="835" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A835" t="s">
+        <v>3043</v>
+      </c>
+      <c r="C835" t="s">
+        <v>2988</v>
+      </c>
+      <c r="D835" t="s">
+        <v>3035</v>
+      </c>
+      <c r="E835" t="s">
+        <v>2959</v>
+      </c>
+      <c r="G835" t="s">
+        <v>3034</v>
+      </c>
+      <c r="AC835" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="836" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A836" t="s">
+        <v>3044</v>
+      </c>
+      <c r="AC836" t="s">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="837" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A837" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B837" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="838" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A838" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B838" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="839" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A839" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B839" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="840" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A840" t="s">
+        <v>3051</v>
+      </c>
+      <c r="B840" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="841" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A841" t="s">
+        <v>3053</v>
+      </c>
+      <c r="B841" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="842" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A842" t="s">
+        <v>3057</v>
+      </c>
+      <c r="B842" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="843" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A843" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B843" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="844" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A844" t="s">
+        <v>3060</v>
+      </c>
+      <c r="B844" t="s">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="845" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A845" t="s">
+        <v>3062</v>
+      </c>
+      <c r="B845" t="s">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="846" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A846" t="s">
+        <v>3063</v>
+      </c>
+      <c r="B846" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="847" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A847" t="s">
+        <v>3065</v>
+      </c>
+      <c r="B847" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="848" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A848" t="s">
+        <v>3069</v>
+      </c>
+      <c r="B848" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A849" t="s">
+        <v>3071</v>
+      </c>
+      <c r="B849" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A850" t="s">
+        <v>3072</v>
+      </c>
+      <c r="B850" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A851" t="s">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A852" t="s">
+        <v>3074</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A853" t="s">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A854" t="s">
+        <v>3076</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A855" t="s">
+        <v>3077</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A856" t="s">
+        <v>3078</v>
+      </c>
+      <c r="B856" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A857" t="s">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A858" t="s">
+        <v>3081</v>
+      </c>
+      <c r="B858" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A859" t="s">
+        <v>3083</v>
+      </c>
+      <c r="B859" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="860" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A860" t="s">
+        <v>3085</v>
+      </c>
+      <c r="B860" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A861" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B861" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A862" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B862" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A863" t="s">
+        <v>3089</v>
+      </c>
+      <c r="B863" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A864" t="s">
+        <v>3091</v>
+      </c>
+    </row>
+    <row r="865" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A865" t="s">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="866" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A866" t="s">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="867" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A867" t="s">
+        <v>3094</v>
+      </c>
+    </row>
+    <row r="868" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A868" t="s">
+        <v>3095</v>
+      </c>
+    </row>
+    <row r="869" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A869" t="s">
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="870" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A870" t="s">
+        <v>3097</v>
+      </c>
+    </row>
+    <row r="871" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A871" t="s">
+        <v>3098</v>
+      </c>
+    </row>
+    <row r="872" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A872" t="s">
+        <v>3099</v>
+      </c>
+    </row>
+    <row r="873" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A873" t="s">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="874" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A874" t="s">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="875" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A875" t="s">
+        <v>3102</v>
+      </c>
+    </row>
+    <row r="876" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A876" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="877" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A877" t="s">
+        <v>3104</v>
+      </c>
+    </row>
+    <row r="878" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A878" t="s">
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="879" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A879" t="s">
+        <v>3106</v>
+      </c>
+    </row>
+    <row r="880" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A880" t="s">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>3109</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>3112</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>3114</v>
+      </c>
+      <c r="B887" t="s">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B888" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>3120</v>
+      </c>
+      <c r="B889" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>3124</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>3127</v>
+      </c>
+      <c r="B895" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>3131</v>
+      </c>
+      <c r="B896" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A897" t="s">
+        <v>3133</v>
+      </c>
+      <c r="B897" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A898" t="s">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A900" t="s">
+        <v>3137</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A901" t="s">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A902" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B903" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B904" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
+        <v>3145</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
+        <v>3148</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A913" t="s">
+        <v>3152</v>
+      </c>
+      <c r="B913" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B914" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A915" t="s">
+        <v>3155</v>
+      </c>
+      <c r="B915" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A916" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B916" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A917" t="s">
+        <v>3159</v>
+      </c>
+      <c r="B917" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A918" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B918" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A919" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B919" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A920" t="s">
+        <v>3164</v>
+      </c>
+      <c r="B920" t="s">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A921" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B921" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A922" t="s">
+        <v>3168</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A923" t="s">
+        <v>3169</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A924" t="s">
+        <v>3170</v>
+      </c>
+      <c r="B924" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A925" t="s">
+        <v>3173</v>
+      </c>
+      <c r="B925" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A926" t="s">
+        <v>3175</v>
+      </c>
+      <c r="B926" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A927" t="s">
+        <v>3177</v>
+      </c>
+      <c r="B927" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A928" t="s">
+        <v>3179</v>
+      </c>
+      <c r="B928" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A929" t="s">
+        <v>3182</v>
+      </c>
+      <c r="B929" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A930" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A931" t="s">
+        <v>3184</v>
+      </c>
+      <c r="B931" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A932" t="s">
+        <v>3186</v>
+      </c>
+      <c r="B932" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A933" t="s">
+        <v>3188</v>
+      </c>
+      <c r="B933" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A934" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B934" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A935" t="s">
+        <v>3192</v>
+      </c>
+      <c r="B935" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A936" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B936" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B937" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A938" t="s">
+        <v>3197</v>
+      </c>
+      <c r="B938" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A939" t="s">
+        <v>3199</v>
+      </c>
+      <c r="B939" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A940" t="s">
+        <v>3200</v>
+      </c>
+      <c r="B940" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B941" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A942" t="s">
+        <v>3203</v>
+      </c>
+      <c r="B942" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A943" t="s">
+        <v>3205</v>
+      </c>
+      <c r="B943" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A944" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A945" t="s">
+        <v>3207</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A946" t="s">
+        <v>3208</v>
+      </c>
+      <c r="B946" t="s">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A947" t="s">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A948" t="s">
+        <v>3186</v>
+      </c>
+      <c r="B948" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A949" t="s">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A950" t="s">
+        <v>3211</v>
+      </c>
+      <c r="B950" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A951" t="s">
+        <v>3213</v>
+      </c>
+      <c r="B951" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A952" t="s">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A953" t="s">
+        <v>3216</v>
+      </c>
+      <c r="B953" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A954" t="s">
+        <v>3218</v>
+      </c>
+      <c r="B954" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A955" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B955" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A956" t="s">
+        <v>3219</v>
+      </c>
+      <c r="B956" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A957" t="s">
+        <v>3221</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A958" t="s">
+        <v>3175</v>
+      </c>
+      <c r="B958" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35949553-CD71-4F74-8474-C85E20024749}">
+  <dimension ref="A1:O144"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D144"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="70" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2943</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2944</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2945</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2946</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2947</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2948</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2949</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>2954</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>2963</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>2954</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>2963</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>2994</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>3002</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>3007</v>
+      </c>
+      <c r="J13" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>3013</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>3020</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>3028</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>3013</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>3048</v>
+      </c>
+      <c r="J24" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>3050</v>
+      </c>
+      <c r="J25" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>3052</v>
+      </c>
+      <c r="J26" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>3055</v>
+      </c>
+      <c r="J27" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>3055</v>
+      </c>
+      <c r="J28" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>3059</v>
+      </c>
+      <c r="J29" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>3061</v>
+      </c>
+      <c r="J30" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>3061</v>
+      </c>
+      <c r="J31" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>3064</v>
+      </c>
+      <c r="J32" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>3067</v>
+      </c>
+      <c r="J33" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>3070</v>
+      </c>
+      <c r="J34" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>3067</v>
+      </c>
+      <c r="J35" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>3070</v>
+      </c>
+      <c r="J36" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>3079</v>
+      </c>
+      <c r="J42" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>3082</v>
+      </c>
+      <c r="J44" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>3084</v>
+      </c>
+      <c r="J45" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>3084</v>
+      </c>
+      <c r="J46" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>3028</v>
+      </c>
+      <c r="J47" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>3088</v>
+      </c>
+      <c r="J48" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>3090</v>
+      </c>
+      <c r="J49" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="73" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>3115</v>
+      </c>
+      <c r="J73" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>3118</v>
+      </c>
+      <c r="J74" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>3121</v>
+      </c>
+      <c r="J75" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>3129</v>
+      </c>
+      <c r="J81" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="82" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>3132</v>
+      </c>
+      <c r="J82" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="83" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>3134</v>
+      </c>
+      <c r="J83" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="89" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>3141</v>
+      </c>
+      <c r="J89" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="90" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>3143</v>
+      </c>
+      <c r="J90" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="99" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>3153</v>
+      </c>
+      <c r="J99" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="100" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>3028</v>
+      </c>
+      <c r="J100" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="101" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>3156</v>
+      </c>
+      <c r="J101" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="102" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>3158</v>
+      </c>
+      <c r="J102" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="103" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>3156</v>
+      </c>
+      <c r="J103" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="104" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>3161</v>
+      </c>
+      <c r="J104" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="105" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>3163</v>
+      </c>
+      <c r="J105" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="106" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>3165</v>
+      </c>
+      <c r="J106" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="107" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>3167</v>
+      </c>
+      <c r="J107" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="110" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>3172</v>
+      </c>
+      <c r="J110" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="111" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>3174</v>
+      </c>
+      <c r="J111" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="112" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>3176</v>
+      </c>
+      <c r="J112" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="113" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>3178</v>
+      </c>
+      <c r="J113" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="114" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>3181</v>
+      </c>
+      <c r="J114" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="115" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>3183</v>
+      </c>
+      <c r="J115" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="117" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>3185</v>
+      </c>
+      <c r="J117" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="118" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>3187</v>
+      </c>
+      <c r="J118" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="119" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>3189</v>
+      </c>
+      <c r="J119" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="120" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>3191</v>
+      </c>
+      <c r="J120" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="121" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>3194</v>
+      </c>
+      <c r="J121" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="122" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>3189</v>
+      </c>
+      <c r="J122" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="123" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>3118</v>
+      </c>
+      <c r="J123" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="124" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>3198</v>
+      </c>
+      <c r="J124" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="125" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>3199</v>
+      </c>
+      <c r="J125" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="126" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>3201</v>
+      </c>
+      <c r="J126" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="127" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>3194</v>
+      </c>
+      <c r="J127" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="128" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>3204</v>
+      </c>
+      <c r="J128" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="129" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>3206</v>
+      </c>
+      <c r="J129" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="132" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>3165</v>
+      </c>
+      <c r="J132" t="s">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="134" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>3187</v>
+      </c>
+      <c r="J134" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="136" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>3212</v>
+      </c>
+      <c r="J136" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="137" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>3214</v>
+      </c>
+      <c r="J137" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="139" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>3217</v>
+      </c>
+      <c r="J139" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="140" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
+        <v>3028</v>
+      </c>
+      <c r="J140" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="141" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>3158</v>
+      </c>
+      <c r="J141" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="142" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>3220</v>
+      </c>
+      <c r="J142" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="144" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>3176</v>
+      </c>
+      <c r="J144" t="s">
+        <v>3171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>